<commit_message>
abgabe ordner weitere sachen eingefügt
</commit_message>
<xml_diff>
--- a/ABGABE_ZIP_ORDNER/Dokumente/UX_Test/Usability_Test_Ergebnisse.xlsx
+++ b/ABGABE_ZIP_ORDNER/Dokumente/UX_Test/Usability_Test_Ergebnisse.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Arbeitsplatz\Studium_Innsbruck\Gerätedesign_Usability\MGST_Geraetedesign-Usability\ABGABE_ZIP_ORDNER\Dokumente\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Arbeitsplatz\Studium_Innsbruck\Gerätedesign_Usability\MGST_Geraetedesign-Usability\ABGABE_ZIP_ORDNER\Dokumente\UX_Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B82F77A7-7554-4212-B405-A1E10CA12696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB6B7F77-3BAD-4069-8EAE-62680B40F545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -184,7 +184,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,16 +200,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -217,17 +230,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="20 % - Akzent5" xfId="1" builtinId="46"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -875,13 +900,13 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17:F20"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="12.86328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.265625" customWidth="1"/>
     <col min="5" max="5" width="31.59765625" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="36.265625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="36.265625" customWidth="1"/>
@@ -889,32 +914,32 @@
     <col min="10" max="10" width="30.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="4" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1323,7 +1348,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1484,20 +1509,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="955644d8-6477-4f1a-a1d1-50fd3035213a" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="955644d8-6477-4f1a-a1d1-50fd3035213a" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1519,25 +1544,25 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{405C8E4F-EE22-4685-89AA-7248B677C43F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="955644d8-6477-4f1a-a1d1-50fd3035213a"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F93E1562-7AE1-458C-8896-56420A321E8D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{405C8E4F-EE22-4685-89AA-7248B677C43F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="955644d8-6477-4f1a-a1d1-50fd3035213a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>